<commit_message>
Finished acceleration with accelerating structure
</commit_message>
<xml_diff>
--- a/Spherical conversions.xlsx
+++ b/Spherical conversions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x15 xr">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="164011"/>
-  <xr:revisionPtr revIDLastSave="27" documentId="{A7D69E28-9E60-4AED-97DD-FE647EB039B9}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="{A7D69E28-9E60-4AED-97DD-FE647EB039B9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
   </bookViews>
@@ -359,8 +359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac xr" xr:uid="{49B971A4-C452-45EB-9755-0FD35E979913}">
   <dimension ref="A1:N113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57:J64"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64:N113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -369,7 +369,7 @@
     <col min="5" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="1.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="2.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2812,7 +2812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="4:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D65">
         <v>3</v>
       </c>
@@ -2830,8 +2830,27 @@
         <f t="shared" si="1"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J65">
+        <v>63</v>
+      </c>
+      <c r="K65">
+        <f t="shared" ref="K65:K113" si="5">ROUND((-1 + SQRT(1 + 4 * N65)) / 2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="L65">
+        <f t="shared" ref="L65:L113" si="6">N65-K65*(K65+1)</f>
+        <v>-3</v>
+      </c>
+      <c r="M65">
+        <f t="shared" ref="M65:M113" si="7">MOD(J65,7)-$B$2</f>
+        <v>-3</v>
+      </c>
+      <c r="N65">
+        <f t="shared" ref="N65:N113" si="8">ROUNDDOWN(J65/(2*$B$2+1),0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D66">
         <v>3</v>
       </c>
@@ -2849,8 +2868,27 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J66">
+        <v>64</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L66">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="M66">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D67">
         <v>3</v>
       </c>
@@ -2861,15 +2899,34 @@
         <v>-1</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G113" si="5">D67*(D67+1)+E67</f>
+        <f t="shared" ref="G67:G113" si="9">D67*(D67+1)+E67</f>
         <v>9</v>
       </c>
       <c r="H67">
-        <f t="shared" ref="H67:H113" si="6">(D67*(D67+1)+E67)*(2*$B$2+1)+F67+$B$2</f>
+        <f t="shared" ref="H67:H113" si="10">(D67*(D67+1)+E67)*(2*$B$2+1)+F67+$B$2</f>
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J67">
+        <v>65</v>
+      </c>
+      <c r="K67">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L67">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="M67">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D68">
         <v>3</v>
       </c>
@@ -2880,15 +2937,34 @@
         <v>0</v>
       </c>
       <c r="G68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="H68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J68">
+        <v>66</v>
+      </c>
+      <c r="K68">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L68">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="M68">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N68">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D69">
         <v>3</v>
       </c>
@@ -2899,15 +2975,34 @@
         <v>1</v>
       </c>
       <c r="G69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="H69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J69">
+        <v>67</v>
+      </c>
+      <c r="K69">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L69">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="M69">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N69">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="70" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D70">
         <v>3</v>
       </c>
@@ -2918,15 +3013,34 @@
         <v>2</v>
       </c>
       <c r="G70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="H70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J70">
+        <v>68</v>
+      </c>
+      <c r="K70">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L70">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="M70">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N70">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="71" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D71">
         <v>3</v>
       </c>
@@ -2937,15 +3051,34 @@
         <v>3</v>
       </c>
       <c r="G71">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="H71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J71">
+        <v>69</v>
+      </c>
+      <c r="K71">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L71">
+        <f t="shared" si="6"/>
+        <v>-3</v>
+      </c>
+      <c r="M71">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N71">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D72">
         <v>3</v>
       </c>
@@ -2956,15 +3089,34 @@
         <v>-3</v>
       </c>
       <c r="G72">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="H72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J72">
+        <v>70</v>
+      </c>
+      <c r="K72">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L72">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="M72">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="N72">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D73">
         <v>3</v>
       </c>
@@ -2975,15 +3127,34 @@
         <v>-2</v>
       </c>
       <c r="G73">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="H73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J73">
+        <v>71</v>
+      </c>
+      <c r="K73">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L73">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D74">
         <v>3</v>
       </c>
@@ -2994,15 +3165,34 @@
         <v>-1</v>
       </c>
       <c r="G74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="H74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="75" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J74">
+        <v>72</v>
+      </c>
+      <c r="K74">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L74">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="M74">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="N74">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D75">
         <v>3</v>
       </c>
@@ -3013,15 +3203,34 @@
         <v>0</v>
       </c>
       <c r="G75">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="H75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>73</v>
       </c>
-    </row>
-    <row r="76" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J75">
+        <v>73</v>
+      </c>
+      <c r="K75">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L75">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="M75">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D76">
         <v>3</v>
       </c>
@@ -3032,15 +3241,34 @@
         <v>1</v>
       </c>
       <c r="G76">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="H76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>74</v>
       </c>
-    </row>
-    <row r="77" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J76">
+        <v>74</v>
+      </c>
+      <c r="K76">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L76">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="M76">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N76">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D77">
         <v>3</v>
       </c>
@@ -3051,15 +3279,34 @@
         <v>2</v>
       </c>
       <c r="G77">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="H77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>75</v>
       </c>
-    </row>
-    <row r="78" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J77">
+        <v>75</v>
+      </c>
+      <c r="K77">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L77">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="M77">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N77">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D78">
         <v>3</v>
       </c>
@@ -3070,15 +3317,34 @@
         <v>3</v>
       </c>
       <c r="G78">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="H78">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J78">
+        <v>76</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L78">
+        <f t="shared" si="6"/>
+        <v>-2</v>
+      </c>
+      <c r="M78">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N78">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D79">
         <v>3</v>
       </c>
@@ -3089,15 +3355,34 @@
         <v>-3</v>
       </c>
       <c r="G79">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="H79">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="80" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J79">
+        <v>77</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L79">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="M79">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="N79">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D80">
         <v>3</v>
       </c>
@@ -3108,15 +3393,34 @@
         <v>-2</v>
       </c>
       <c r="G80">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="H80">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="81" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J80">
+        <v>78</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L80">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="M80">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="N80">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D81">
         <v>3</v>
       </c>
@@ -3127,15 +3431,34 @@
         <v>-1</v>
       </c>
       <c r="G81">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="H81">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="82" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J81">
+        <v>79</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L81">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="M81">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="N81">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D82">
         <v>3</v>
       </c>
@@ -3146,15 +3469,34 @@
         <v>0</v>
       </c>
       <c r="G82">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="H82">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="83" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J82">
+        <v>80</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L82">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="M82">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N82">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D83">
         <v>3</v>
       </c>
@@ -3165,15 +3507,34 @@
         <v>1</v>
       </c>
       <c r="G83">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="H83">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J83">
+        <v>81</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L83">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="M83">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N83">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D84">
         <v>3</v>
       </c>
@@ -3184,15 +3545,34 @@
         <v>2</v>
       </c>
       <c r="G84">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="H84">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="85" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J84">
+        <v>82</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L84">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="M84">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N84">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D85">
         <v>3</v>
       </c>
@@ -3203,15 +3583,34 @@
         <v>3</v>
       </c>
       <c r="G85">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="H85">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="86" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J85">
+        <v>83</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L85">
+        <f t="shared" si="6"/>
+        <v>-1</v>
+      </c>
+      <c r="M85">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N85">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D86">
         <v>3</v>
       </c>
@@ -3222,15 +3621,34 @@
         <v>-3</v>
       </c>
       <c r="G86">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="H86">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="87" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J86">
+        <v>84</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L86">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="N86">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D87">
         <v>3</v>
       </c>
@@ -3241,15 +3659,34 @@
         <v>-2</v>
       </c>
       <c r="G87">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="H87">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="88" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J87">
+        <v>85</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L87">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="N87">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D88">
         <v>3</v>
       </c>
@@ -3260,15 +3697,34 @@
         <v>-1</v>
       </c>
       <c r="G88">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="H88">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="89" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J88">
+        <v>86</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L88">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="N88">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D89">
         <v>3</v>
       </c>
@@ -3279,15 +3735,34 @@
         <v>0</v>
       </c>
       <c r="G89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="H89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="90" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J89">
+        <v>87</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L89">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N89">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="90" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D90">
         <v>3</v>
       </c>
@@ -3298,15 +3773,34 @@
         <v>1</v>
       </c>
       <c r="G90">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="H90">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="91" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J90">
+        <v>88</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L90">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N90">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D91">
         <v>3</v>
       </c>
@@ -3317,15 +3811,34 @@
         <v>2</v>
       </c>
       <c r="G91">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="H91">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="92" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J91">
+        <v>89</v>
+      </c>
+      <c r="K91">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L91">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M91">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N91">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D92">
         <v>3</v>
       </c>
@@ -3336,15 +3849,34 @@
         <v>3</v>
       </c>
       <c r="G92">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="H92">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="93" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J92">
+        <v>90</v>
+      </c>
+      <c r="K92">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L92">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N92">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D93">
         <v>3</v>
       </c>
@@ -3355,15 +3887,34 @@
         <v>-3</v>
       </c>
       <c r="G93">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="H93">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="94" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J93">
+        <v>91</v>
+      </c>
+      <c r="K93">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L93">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M93">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="N93">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D94">
         <v>3</v>
       </c>
@@ -3374,15 +3925,34 @@
         <v>-2</v>
       </c>
       <c r="G94">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="H94">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="95" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J94">
+        <v>92</v>
+      </c>
+      <c r="K94">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L94">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M94">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="N94">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D95">
         <v>3</v>
       </c>
@@ -3393,15 +3963,34 @@
         <v>-1</v>
       </c>
       <c r="G95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="H95">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="96" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J95">
+        <v>93</v>
+      </c>
+      <c r="K95">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L95">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M95">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="N95">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="96" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D96">
         <v>3</v>
       </c>
@@ -3412,15 +4001,34 @@
         <v>0</v>
       </c>
       <c r="G96">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="H96">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="97" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J96">
+        <v>94</v>
+      </c>
+      <c r="K96">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L96">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M96">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N96">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D97">
         <v>3</v>
       </c>
@@ -3431,15 +4039,34 @@
         <v>1</v>
       </c>
       <c r="G97">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="H97">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="98" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J97">
+        <v>95</v>
+      </c>
+      <c r="K97">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L97">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M97">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N97">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="98" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D98">
         <v>3</v>
       </c>
@@ -3450,15 +4077,34 @@
         <v>2</v>
       </c>
       <c r="G98">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="H98">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="99" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J98">
+        <v>96</v>
+      </c>
+      <c r="K98">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L98">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M98">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N98">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D99">
         <v>3</v>
       </c>
@@ -3469,15 +4115,34 @@
         <v>3</v>
       </c>
       <c r="G99">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="H99">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>97</v>
       </c>
-    </row>
-    <row r="100" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J99">
+        <v>97</v>
+      </c>
+      <c r="K99">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L99">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M99">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N99">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D100">
         <v>3</v>
       </c>
@@ -3488,15 +4153,34 @@
         <v>-3</v>
       </c>
       <c r="G100">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="H100">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="101" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J100">
+        <v>98</v>
+      </c>
+      <c r="K100">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L100">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M100">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="N100">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D101">
         <v>3</v>
       </c>
@@ -3507,15 +4191,34 @@
         <v>-2</v>
       </c>
       <c r="G101">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="H101">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="102" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J101">
+        <v>99</v>
+      </c>
+      <c r="K101">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L101">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M101">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="N101">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D102">
         <v>3</v>
       </c>
@@ -3526,15 +4229,34 @@
         <v>-1</v>
       </c>
       <c r="G102">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="H102">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="103" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J102">
+        <v>100</v>
+      </c>
+      <c r="K102">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L102">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M102">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="N102">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D103">
         <v>3</v>
       </c>
@@ -3545,15 +4267,34 @@
         <v>0</v>
       </c>
       <c r="G103">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="H103">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>101</v>
       </c>
-    </row>
-    <row r="104" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J103">
+        <v>101</v>
+      </c>
+      <c r="K103">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L103">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M103">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N103">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D104">
         <v>3</v>
       </c>
@@ -3564,15 +4305,34 @@
         <v>1</v>
       </c>
       <c r="G104">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="H104">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>102</v>
       </c>
-    </row>
-    <row r="105" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J104">
+        <v>102</v>
+      </c>
+      <c r="K104">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L104">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M104">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N104">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D105">
         <v>3</v>
       </c>
@@ -3583,15 +4343,34 @@
         <v>2</v>
       </c>
       <c r="G105">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="H105">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>103</v>
       </c>
-    </row>
-    <row r="106" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J105">
+        <v>103</v>
+      </c>
+      <c r="K105">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L105">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M105">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N105">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D106">
         <v>3</v>
       </c>
@@ -3602,15 +4381,34 @@
         <v>3</v>
       </c>
       <c r="G106">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="H106">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>104</v>
       </c>
-    </row>
-    <row r="107" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J106">
+        <v>104</v>
+      </c>
+      <c r="K106">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L106">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="M106">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N106">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D107">
         <v>3</v>
       </c>
@@ -3621,15 +4419,34 @@
         <v>-3</v>
       </c>
       <c r="G107">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="H107">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="108" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J107">
+        <v>105</v>
+      </c>
+      <c r="K107">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L107">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="M107">
+        <f t="shared" si="7"/>
+        <v>-3</v>
+      </c>
+      <c r="N107">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D108">
         <v>3</v>
       </c>
@@ -3640,15 +4457,34 @@
         <v>-2</v>
       </c>
       <c r="G108">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="H108">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J108">
+        <v>106</v>
+      </c>
+      <c r="K108">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L108">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="M108">
+        <f t="shared" si="7"/>
+        <v>-2</v>
+      </c>
+      <c r="N108">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D109">
         <v>3</v>
       </c>
@@ -3659,15 +4495,34 @@
         <v>-1</v>
       </c>
       <c r="G109">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="H109">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>107</v>
       </c>
-    </row>
-    <row r="110" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J109">
+        <v>107</v>
+      </c>
+      <c r="K109">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L109">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="M109">
+        <f t="shared" si="7"/>
+        <v>-1</v>
+      </c>
+      <c r="N109">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D110">
         <v>3</v>
       </c>
@@ -3678,15 +4533,34 @@
         <v>0</v>
       </c>
       <c r="G110">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="H110">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>108</v>
       </c>
-    </row>
-    <row r="111" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J110">
+        <v>108</v>
+      </c>
+      <c r="K110">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L110">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="M110">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N110">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D111">
         <v>3</v>
       </c>
@@ -3697,15 +4571,34 @@
         <v>1</v>
       </c>
       <c r="G111">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="H111">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>109</v>
       </c>
-    </row>
-    <row r="112" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J111">
+        <v>109</v>
+      </c>
+      <c r="K111">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L111">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="M111">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N111">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D112">
         <v>3</v>
       </c>
@@ -3716,15 +4609,34 @@
         <v>2</v>
       </c>
       <c r="G112">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="H112">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>110</v>
       </c>
-    </row>
-    <row r="113" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="J112">
+        <v>110</v>
+      </c>
+      <c r="K112">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L112">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="M112">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="N112">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D113">
         <v>3</v>
       </c>
@@ -3735,12 +4647,31 @@
         <v>3</v>
       </c>
       <c r="G113">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="H113">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>111</v>
+      </c>
+      <c r="J113">
+        <v>111</v>
+      </c>
+      <c r="K113">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="L113">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="M113">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N113">
+        <f t="shared" si="8"/>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>